<commit_message>
chore: contamination, delete segmented models, replace by spearman's tests => tributyltin
</commit_message>
<xml_diff>
--- a/inst/results/data_contam/tributyltin/summarised_levels_data_tributyltin_dw.xlsx
+++ b/inst/results/data_contam/tributyltin/summarised_levels_data_tributyltin_dw.xlsx
@@ -387,7 +387,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Tributylétain cation</t>
+          <t>Tributyltin cation</t>
         </is>
       </c>
       <c r="C2">
@@ -405,7 +405,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Tributylétain cation</t>
+          <t>Tributyltin cation</t>
         </is>
       </c>
       <c r="C3">
@@ -423,7 +423,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tributylétain cation</t>
+          <t>Tributyltin cation</t>
         </is>
       </c>
       <c r="C4">

</xml_diff>